<commit_message>
untuk menambahkan input email alumni
</commit_message>
<xml_diff>
--- a/public/template_alumni.xlsx
+++ b/public/template_alumni.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PBL_TracerStudy\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC287D0E-70F1-47D1-A644-0AD7FD4003AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F8E74C-DA88-48B2-ADD8-3A918C0AB2CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="8880" xr2:uid="{1AE5AECB-4DC8-4DAA-BF18-2A05E6D573E0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Prodi</t>
   </si>
@@ -43,16 +43,30 @@
   </si>
   <si>
     <t>Naafi' Ridho Athallah</t>
+  </si>
+  <si>
+    <t>naafiridho0505@gmail.com</t>
+  </si>
+  <si>
+    <t>Email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,14 +89,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -395,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC702BD1-04C8-481E-923E-39CF5E5B158A}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -407,9 +424,10 @@
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="14.5546875" customWidth="1"/>
     <col min="4" max="4" width="17.21875" customWidth="1"/>
+    <col min="5" max="5" width="24.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -422,8 +440,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -436,8 +457,14 @@
       <c r="D2" s="1">
         <v>45153</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{74206FB0-1A86-417F-89C4-0ECD9787922C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>